<commit_message>
load of MDDW & MAD stuff
</commit_message>
<xml_diff>
--- a/questionnaires/RBDstandardized_questionnaireMDDW_FR.xlsx
+++ b/questionnaires/RBDstandardized_questionnaireMDDW_FR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RBD_Resilience_guide_FR\questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F3320C-A889-4C05-B5A3-23E71B92D087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1329E7-C110-4312-8363-98541F71F53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1545" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>Nom et prénom de la femme (No ${HHSize1549F_MDDW_calc})</t>
   </si>
   <si>
-    <t>Age en années révolues de ${MDDW_resp_age}</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>Francais</t>
+  </si>
+  <si>
+    <t>Age en années révolues de ${MDDW_name}</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1576,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1656,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>76</v>
       </c>
       <c r="E6" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,10 +1705,10 @@
         <v>75</v>
       </c>
       <c r="C7" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="65" t="s">
         <v>77</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>78</v>
       </c>
       <c r="F7" s="68" t="s">
         <v>58</v>
@@ -1725,10 +1725,10 @@
         <v>60</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1739,13 +1739,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1756,13 +1756,13 @@
         <v>26</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1773,13 +1773,13 @@
         <v>35</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="70"/>
       <c r="J11" s="67"/>
@@ -1792,13 +1792,13 @@
         <v>36</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="67"/>
       <c r="J12" s="70"/>
@@ -1811,13 +1811,13 @@
         <v>37</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="67"/>
       <c r="J13" s="70"/>
@@ -1830,13 +1830,13 @@
         <v>31</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="66" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -1847,13 +1847,13 @@
         <v>32</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" s="70"/>
       <c r="J15" s="67"/>
@@ -1869,10 +1869,10 @@
         <v>47</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="67"/>
       <c r="J16" s="70"/>
@@ -1885,13 +1885,13 @@
         <v>33</v>
       </c>
       <c r="C17" s="61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="67"/>
       <c r="J17" s="70"/>
@@ -1904,13 +1904,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J18" s="69"/>
     </row>
@@ -1922,13 +1922,13 @@
         <v>27</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J19" s="69"/>
     </row>
@@ -1940,13 +1940,13 @@
         <v>29</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1957,13 +1957,13 @@
         <v>28</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E21" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,13 +1974,13 @@
         <v>30</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E22" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="66" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1991,13 +1991,13 @@
         <v>38</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F23" s="70"/>
       <c r="J23" s="67"/>
@@ -2010,13 +2010,13 @@
         <v>39</v>
       </c>
       <c r="C24" s="61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24" s="67"/>
       <c r="J24" s="70"/>
@@ -2029,13 +2029,13 @@
         <v>44</v>
       </c>
       <c r="C25" s="61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="67"/>
       <c r="J25" s="70"/>
@@ -2067,7 +2067,7 @@
         <v>61</v>
       </c>
       <c r="E27" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" s="70"/>
       <c r="J27" s="70"/>
@@ -2083,7 +2083,7 @@
         <v>62</v>
       </c>
       <c r="E28" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F28" s="69"/>
       <c r="J28" s="69"/>
@@ -2099,7 +2099,7 @@
         <v>63</v>
       </c>
       <c r="E29" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J29" s="69"/>
     </row>
@@ -2114,7 +2114,7 @@
         <v>64</v>
       </c>
       <c r="E30" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J30" s="69"/>
     </row>
@@ -2129,7 +2129,7 @@
         <v>65</v>
       </c>
       <c r="E31" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F31" s="69"/>
       <c r="J31" s="69"/>
@@ -2145,7 +2145,7 @@
         <v>66</v>
       </c>
       <c r="E32" s="65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J32" s="69"/>
     </row>
@@ -5227,7 +5227,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5249,21 +5249,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D9E21B46B6510944ACCC1A9E9D09B45B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b02bb79e95f874242395453643404308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0aae8104-2775-47bf-a616-40d8eadd5188" xmlns:ns4="8dd5283b-55c2-4f3c-990c-ab18dea8320e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d6c59ce88ebf0eb87405994d35ea81e" ns3:_="" ns4:_="">
     <xsd:import namespace="0aae8104-2775-47bf-a616-40d8eadd5188"/>
@@ -5480,32 +5465,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50755B8E-7E00-4BEC-BA51-4E6E4B22BCE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0aae8104-2775-47bf-a616-40d8eadd5188"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8dd5283b-55c2-4f3c-990c-ab18dea8320e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D66C5643-24C7-4807-886B-BE44B695FAF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF46C5BC-2557-46C4-92CA-B3C69F93D2EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5522,4 +5497,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D66C5643-24C7-4807-886B-BE44B695FAF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50755B8E-7E00-4BEC-BA51-4E6E4B22BCE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0aae8104-2775-47bf-a616-40d8eadd5188"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8dd5283b-55c2-4f3c-990c-ab18dea8320e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>